<commit_message>
Show template - result pairs in the readme
Should help users find the right example more easily.
</commit_message>
<xml_diff>
--- a/Advanced/SheetReport (Java)/src/main/resources/Report.xlsx
+++ b/Advanced/SheetReport (Java)/src/main/resources/Report.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="645" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -137,6 +137,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="hr-HR"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:perspective val="30"/>
@@ -172,16 +173,18 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls/>
       </c:pie3DChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -268,7 +271,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Author" refreshedDate="42833.820988888889" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Author" refreshedDate="42945.799522222223" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
@@ -307,7 +310,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="645" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B4:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -679,7 +682,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>